<commit_message>
Format Update for Aesthetics
</commit_message>
<xml_diff>
--- a/Documents/RTM.xlsx
+++ b/Documents/RTM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\team6\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B9C53F-A9FF-4B11-B14D-F17B729F6AF1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E74EBC5-DC8C-4285-B4C7-8A591183AE79}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,25 +550,25 @@
   <dimension ref="A1:J300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" style="3" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="3" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="55.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>